<commit_message>
final version working, no email sender
</commit_message>
<xml_diff>
--- a/data/test_sheet.xlsx
+++ b/data/test_sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26212"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2B8C353-8359-4ACE-A84C-3C8E37C86E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{823456E6-ABB3-4A71-A724-D510583B2C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,27 +28,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
-  <si>
-    <t>SEQUENCIAL</t>
-  </si>
-  <si>
-    <t>NUMERO EQUIPAMENTO</t>
-  </si>
-  <si>
-    <t>Sigla SE</t>
-  </si>
-  <si>
-    <t>Tipo equip</t>
-  </si>
-  <si>
-    <t>Operacional</t>
-  </si>
-  <si>
-    <t>Data da Troca da Bateria</t>
-  </si>
-  <si>
-    <t>300-05757</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+  <si>
+    <t>sigla_se</t>
+  </si>
+  <si>
+    <t>tipo_equip</t>
+  </si>
+  <si>
+    <t>operacional</t>
+  </si>
+  <si>
+    <t>data_ultima_troca</t>
+  </si>
+  <si>
+    <t>data_proxima_troca</t>
   </si>
   <si>
     <t xml:space="preserve">GUA </t>
@@ -60,7 +54,7 @@
     <t xml:space="preserve"> 83972CPN02</t>
   </si>
   <si>
-    <t>300-05770</t>
+    <t xml:space="preserve"> 14/06/2021</t>
   </si>
   <si>
     <t xml:space="preserve">SRG </t>
@@ -69,7 +63,7 @@
     <t xml:space="preserve"> 83972CTU02</t>
   </si>
   <si>
-    <t>300-05781</t>
+    <t xml:space="preserve"> 27/04/2022</t>
   </si>
   <si>
     <t xml:space="preserve">MOT </t>
@@ -78,7 +72,7 @@
     <t xml:space="preserve"> 83972BUR01</t>
   </si>
   <si>
-    <t>300-06116</t>
+    <t xml:space="preserve"> 20/02/2020</t>
   </si>
   <si>
     <t xml:space="preserve">BTA </t>
@@ -90,9 +84,6 @@
     <t xml:space="preserve"> 11/07/2018</t>
   </si>
   <si>
-    <t>300-06118</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAS </t>
   </si>
   <si>
@@ -102,30 +93,18 @@
     <t xml:space="preserve"> 15/06/2021</t>
   </si>
   <si>
-    <t>300-06123</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 83972VRI01</t>
   </si>
   <si>
     <t xml:space="preserve"> 14/04/2022</t>
   </si>
   <si>
-    <t>300-06126</t>
-  </si>
-  <si>
     <t xml:space="preserve">BIT </t>
   </si>
   <si>
     <t xml:space="preserve"> 89432SAO01</t>
   </si>
   <si>
-    <t xml:space="preserve"> 14/06/2021</t>
-  </si>
-  <si>
-    <t>300-06133</t>
-  </si>
-  <si>
     <t xml:space="preserve">PIN </t>
   </si>
   <si>
@@ -135,15 +114,9 @@
     <t xml:space="preserve"> 19/05/2021</t>
   </si>
   <si>
-    <t>300-06220</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 27/05/2021</t>
   </si>
   <si>
-    <t>300-06229</t>
-  </si>
-  <si>
     <t xml:space="preserve">IBU </t>
   </si>
   <si>
@@ -151,46 +124,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>300-06232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SJC </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 83972SVH01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16/06/2021</t>
-  </si>
-  <si>
-    <t>300-06236</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 86696SRT01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12/07/2021</t>
-  </si>
-  <si>
-    <t>300-06249</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 83972TAQ01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 18/05/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="165" formatCode="d/m;@"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -220,18 +159,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,18 +478,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,16 +497,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>176961</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -592,252 +514,131 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3">
-        <v>44361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>107898</v>
-      </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3">
-        <v>44678</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>150177</v>
-      </c>
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3">
-        <f>DATEVALUE("20/02/2020")</f>
-        <v>43881</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>134410</v>
-      </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>118711</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>131505</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>134376</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>135016</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>118650</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>121743</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>137419</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>121742</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>158487</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>